<commit_message>
Ajout version 2 Parduzi SecureSign mail bdd bailleur
</commit_message>
<xml_diff>
--- a/parduzi_app/server/templates/parduzi_standard.xlsx
+++ b/parduzi_app/server/templates/parduzi_standard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Beni\travail partage\AAAA TABLEAU\HMP BOIS - MARCHE 2021-055\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erion\Desktop\parduzi secursign\parduzi_app\server\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BCBBF6-B76D-4DB4-807A-82C5C2A79CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9219409-9BA6-4246-97A6-146A6961DB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quitus" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t xml:space="preserve">     </t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">DATE : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBJET : </t>
   </si>
   <si>
     <t xml:space="preserve">    LE CLIENT  ou  GARDIEN </t>
@@ -116,6 +113,15 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>BAILLEUR :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMARQUES : </t>
+  </si>
+  <si>
+    <t>N° interne :</t>
   </si>
 </sst>
 </file>
@@ -375,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,6 +461,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -533,13 +542,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -582,77 +591,6 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1590675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="ZoneTexte 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{364973AD-9448-40B5-BE0D-1F40BD8AEB6E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2000250" y="4391025"/>
-          <a:ext cx="3771900" cy="2933700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>REMARQUES</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -999,217 +937,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F1" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="16">
-        <v>2025</v>
-      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="13" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+    <row r="15" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="16"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="12" t="s">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:17" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:17" ht="24.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="B19" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="12"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="Q20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:17" ht="24.9" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A21" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="19" t="s">
+      <c r="Q21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="24.9" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="4"/>
-      <c r="B23" s="10"/>
+    <row r="23" spans="1:17" ht="24.9" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:17" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -1217,57 +1157,65 @@
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:17" ht="126.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="13"/>
+    <row r="25" spans="1:17" ht="18.600000000000001" x14ac:dyDescent="0.45">
+      <c r="A25" s="4"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:17" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:17" ht="101.4" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="13"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:17" ht="18.600000000000001" x14ac:dyDescent="0.45">
+      <c r="A27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:17" ht="18.600000000000001" x14ac:dyDescent="0.45">
+      <c r="A28" s="12"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:17" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="E31" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="E30" s="5" t="s">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1225,7 @@
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A10:F10"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -1291,88 +1239,88 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-    </row>
-    <row r="11" spans="1:7" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+    </row>
+    <row r="11" spans="1:7" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25"/>
       <c r="B12" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="27"/>
     </row>
-    <row r="13" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="10" t="s">
         <v>4</v>
@@ -1382,9 +1330,9 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
@@ -1392,17 +1340,17 @@
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
     </row>
-    <row r="15" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="29"/>
       <c r="B15" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="30" t="s">
         <v>4</v>
@@ -1412,9 +1360,9 @@
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -1422,7 +1370,7 @@
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
     </row>
-    <row r="18" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
       <c r="B18" s="30" t="s">
         <v>4</v>
@@ -1432,9 +1380,9 @@
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
@@ -1442,7 +1390,7 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
-    <row r="20" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="10" t="s">
         <v>4</v>
@@ -1456,7 +1404,7 @@
       </c>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="12"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -1464,14 +1412,14 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A22" s="11"/>
       <c r="B22" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A23" s="11"/>
       <c r="B23" s="23" t="s">
         <v>4</v>
@@ -1481,7 +1429,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A24" s="20"/>
       <c r="B24" s="23" t="s">
         <v>4</v>
@@ -1491,7 +1439,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -1499,7 +1447,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1507,7 +1455,7 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" s="13"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -1515,7 +1463,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:6" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A28" s="12"/>
       <c r="B28" s="10"/>
       <c r="C28" s="24" t="s">
@@ -1525,7 +1473,7 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:6" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A29" s="12"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -1533,7 +1481,7 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:6" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A30" s="12"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1541,7 +1489,7 @@
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:6" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1549,7 +1497,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:6" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A32" s="4"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1557,24 +1505,24 @@
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="E37" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +1544,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1608,7 +1556,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>